<commit_message>
qaz v1.1: fixes going from v1.0->v1.1
Changed from individual pull up/down on BOOT0 MCU pin to switch that can
easily change from one to the other (without soldering). This is
required for programming over USB DFU.

Fixed RESET switch, pins were flipped on part layout.
</commit_message>
<xml_diff>
--- a/hardware/QAZ_65/pcb/QAZ_65/QAZ_65_1v0_BOM.xlsx
+++ b/hardware/QAZ_65/pcb/QAZ_65/QAZ_65_1v0_BOM.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opt\QAZ\hardware\QAZ_65\pcb\QAZ_65\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\opt\qaz\hardware\QAZ_65\pcb\QAZ_65\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B8B70F-5865-4493-AD52-EE4CBCAD2249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="119">
   <si>
     <t>BOM Index</t>
   </si>
@@ -368,9 +367,6 @@
     <t>R14, R17</t>
   </si>
   <si>
-    <t>R1, R2, R15, R16</t>
-  </si>
-  <si>
     <t>R10, R11</t>
   </si>
   <si>
@@ -381,12 +377,27 @@
   </si>
   <si>
     <t>"Available"</t>
+  </si>
+  <si>
+    <t>R2, R15, R16</t>
+  </si>
+  <si>
+    <t>JS102011SCQN</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>SW70</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/JS102011SCQN/3753547</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
@@ -519,7 +530,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -598,6 +609,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -981,7 +993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -999,14 +1011,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ62"/>
+  <dimension ref="A1:AMJ63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" activeCellId="1" sqref="D27 H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L2" s="7"/>
     </row>
@@ -1071,14 +1083,14 @@
         <v>10</v>
       </c>
       <c r="E3" s="8">
-        <f t="shared" ref="E3:E28" si="0">LEN(TRIM(H3))-LEN(SUBSTITUTE(TRIM(H3),",",""))+1</f>
+        <f>LEN(TRIM(H3))-LEN(SUBSTITUTE(TRIM(H3),",",""))+1</f>
         <v>6</v>
       </c>
       <c r="F3" s="11">
         <v>0.1</v>
       </c>
       <c r="G3" s="11">
-        <f t="shared" ref="G3:G22" si="1">E3*F3</f>
+        <f>E3*F3</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="H3" s="22" t="s">
@@ -1095,7 +1107,7 @@
     </row>
     <row r="4" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
-        <f t="shared" ref="B4:B28" si="2">B3+1</f>
+        <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -1105,14 +1117,14 @@
         <v>16</v>
       </c>
       <c r="E4" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H4))-LEN(SUBSTITUTE(TRIM(H4),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F4" s="11">
         <v>0.17</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" si="1"/>
+        <f>E4*F4</f>
         <v>0.17</v>
       </c>
       <c r="H4" s="22" t="s">
@@ -1129,7 +1141,7 @@
     </row>
     <row r="5" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
-        <f t="shared" si="2"/>
+        <f>B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1139,14 +1151,14 @@
         <v>19</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H5))-LEN(SUBSTITUTE(TRIM(H5),",",""))+1</f>
         <v>4</v>
       </c>
       <c r="F5" s="11">
         <v>0.1</v>
       </c>
       <c r="G5" s="11">
-        <f t="shared" si="1"/>
+        <f>E5*F5</f>
         <v>0.4</v>
       </c>
       <c r="H5" s="22" t="s">
@@ -1163,7 +1175,7 @@
     </row>
     <row r="6" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
-        <f t="shared" si="2"/>
+        <f>B5+1</f>
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1173,14 +1185,14 @@
         <v>13</v>
       </c>
       <c r="E6" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H6))-LEN(SUBSTITUTE(TRIM(H6),",",""))+1</f>
         <v>2</v>
       </c>
       <c r="F6" s="11">
         <v>0.1</v>
       </c>
       <c r="G6" s="11">
-        <f t="shared" si="1"/>
+        <f>E6*F6</f>
         <v>0.2</v>
       </c>
       <c r="H6" s="22" t="s">
@@ -1197,7 +1209,7 @@
     </row>
     <row r="7" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
-        <f t="shared" si="2"/>
+        <f>B6+1</f>
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1207,14 +1219,14 @@
         <v>22</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H7))-LEN(SUBSTITUTE(TRIM(H7),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F7" s="11">
         <v>1.37</v>
       </c>
       <c r="G7" s="11">
-        <f t="shared" si="1"/>
+        <f>E7*F7</f>
         <v>1.37</v>
       </c>
       <c r="H7" s="22" t="s">
@@ -1236,338 +1248,338 @@
         <f>B7+1</f>
         <v>6</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>94</v>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>LEN(TRIM(H8))-LEN(SUBSTITUTE(TRIM(H8),",",""))+1</f>
+        <v>68</v>
       </c>
       <c r="F8" s="11">
-        <v>0.18</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="G8" s="11">
-        <f t="shared" si="1"/>
-        <v>0.18</v>
+        <f>E8*F8</f>
+        <v>3.9440000000000004</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="12">
-        <v>0</v>
-      </c>
-      <c r="K8" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="I8" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>93</v>
+      </c>
       <c r="L8" s="16"/>
     </row>
     <row r="9" spans="2:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
-        <f t="shared" si="2"/>
+        <f>B8+1</f>
         <v>7</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>24</v>
+      <c r="C9" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="0"/>
-        <v>68</v>
+        <f>LEN(TRIM(H9))-LEN(SUBSTITUTE(TRIM(H9),",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="F9" s="11">
-        <v>5.8000000000000003E-2</v>
+        <v>0.18</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="1"/>
-        <v>3.9440000000000004</v>
+        <f>E9*F9</f>
+        <v>0.18</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>93</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12"/>
       <c r="L9" s="16"/>
     </row>
     <row r="10" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
-        <f t="shared" si="2"/>
+        <f>B9+1</f>
         <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="E10" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H10))-LEN(SUBSTITUTE(TRIM(H10),",",""))+1</f>
+        <v>3</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G10" s="11">
+        <f>E10*F10</f>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="12">
+        <v>2</v>
+      </c>
+      <c r="K10" s="12">
         <v>1</v>
       </c>
-      <c r="F10" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="11">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="J10" s="12">
-        <v>7</v>
-      </c>
-      <c r="K10" s="12"/>
       <c r="L10" s="16"/>
     </row>
     <row r="11" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
-        <f t="shared" si="2"/>
+        <f>B10+1</f>
         <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H11))-LEN(SUBSTITUTE(TRIM(H11),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F11" s="11">
-        <v>0.28000000000000003</v>
+        <v>0.5</v>
       </c>
       <c r="G11" s="11">
-        <f t="shared" si="1"/>
-        <v>0.28000000000000003</v>
+        <f>E11*F11</f>
+        <v>0.5</v>
       </c>
       <c r="H11" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>29</v>
+        <v>33</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="J11" s="12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="16"/>
     </row>
     <row r="12" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
-        <f t="shared" si="2"/>
+        <f>B11+1</f>
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H12))-LEN(SUBSTITUTE(TRIM(H12),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F12" s="11">
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="G12" s="11">
-        <f t="shared" si="1"/>
-        <v>0.26</v>
+        <f>E12*F12</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H12" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J12" s="12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="16"/>
     </row>
     <row r="13" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
-        <f t="shared" si="2"/>
+        <f>B12+1</f>
         <v>11</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>89</v>
+        <v>30</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>LEN(TRIM(H13))-LEN(SUBSTITUTE(TRIM(H13),",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="F13" s="11">
-        <v>0.55000000000000004</v>
+        <v>0.26</v>
       </c>
       <c r="G13" s="11">
-        <f t="shared" si="1"/>
-        <v>1.6500000000000001</v>
+        <f>E13*F13</f>
+        <v>0.26</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="I13" s="29" t="s">
-        <v>91</v>
+        <v>101</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="J13" s="12">
-        <v>2</v>
-      </c>
-      <c r="K13" s="12">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="K13" s="12"/>
       <c r="L13" s="16"/>
     </row>
     <row r="14" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
-        <f t="shared" si="2"/>
+        <f>B13+1</f>
         <v>12</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E14" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>LEN(TRIM(H14))-LEN(SUBSTITUTE(TRIM(H14),",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="F14" s="11">
         <v>0.1</v>
       </c>
       <c r="G14" s="11">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
+        <f>E14*F14</f>
+        <v>0.2</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>46</v>
+        <v>110</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>87</v>
       </c>
       <c r="J14" s="12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K14" s="12"/>
       <c r="L14" s="16"/>
     </row>
     <row r="15" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
-        <f t="shared" si="2"/>
+        <f>B14+1</f>
         <v>13</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H15))-LEN(SUBSTITUTE(TRIM(H15),",",""))+1</f>
         <v>2</v>
       </c>
       <c r="F15" s="11">
         <v>0.1</v>
       </c>
       <c r="G15" s="11">
-        <f t="shared" si="1"/>
+        <f>E15*F15</f>
         <v>0.2</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>39</v>
+        <v>111</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="J15" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K15" s="12"/>
       <c r="L15" s="16"/>
     </row>
     <row r="16" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
-        <f t="shared" si="2"/>
+        <f>B15+1</f>
         <v>14</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>LEN(TRIM(H16))-LEN(SUBSTITUTE(TRIM(H16),",",""))+1</f>
+        <v>2</v>
       </c>
       <c r="F16" s="11">
         <v>0.1</v>
       </c>
       <c r="G16" s="11">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f>E16*F16</f>
+        <v>0.2</v>
       </c>
       <c r="H16" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J16" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K16" s="12"/>
       <c r="L16" s="16"/>
     </row>
     <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
-        <f t="shared" si="2"/>
+        <f>B16+1</f>
         <v>15</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>LEN(TRIM(H17))-LEN(SUBSTITUTE(TRIM(H17),",",""))+1</f>
+        <v>3</v>
       </c>
       <c r="F17" s="11">
         <v>0.1</v>
       </c>
       <c r="G17" s="11">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f>E17*F17</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="29" t="s">
-        <v>87</v>
+        <v>114</v>
+      </c>
+      <c r="I17" s="24" t="s">
+        <v>36</v>
       </c>
       <c r="J17" s="12">
         <v>8</v>
@@ -1577,109 +1589,109 @@
     </row>
     <row r="18" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
-        <f t="shared" si="2"/>
+        <f>B17+1</f>
         <v>16</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E18" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>LEN(TRIM(H18))-LEN(SUBSTITUTE(TRIM(H18),",",""))+1</f>
+        <v>5</v>
       </c>
       <c r="F18" s="11">
         <v>0.1</v>
       </c>
       <c r="G18" s="11">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
+        <f>E18*F18</f>
+        <v>0.5</v>
       </c>
       <c r="H18" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>69</v>
+        <v>112</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="J18" s="12">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K18" s="12"/>
       <c r="L18" s="16"/>
     </row>
     <row r="19" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
-        <f t="shared" si="2"/>
+        <f>B18+1</f>
         <v>17</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="E19" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>LEN(TRIM(H19))-LEN(SUBSTITUTE(TRIM(H19),",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="F19" s="11">
         <v>0.1</v>
       </c>
       <c r="G19" s="11">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+        <f>E19*F19</f>
+        <v>0.1</v>
       </c>
       <c r="H19" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="J19" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K19" s="12"/>
       <c r="L19" s="16"/>
     </row>
     <row r="20" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
-        <f t="shared" si="2"/>
+        <f>B19+1</f>
         <v>18</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="E20" s="8">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>LEN(TRIM(H20))-LEN(SUBSTITUTE(TRIM(H20),",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="F20" s="11">
         <v>0.1</v>
       </c>
       <c r="G20" s="11">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f>E20*F20</f>
+        <v>0.1</v>
       </c>
       <c r="H20" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>43</v>
+        <v>108</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>69</v>
       </c>
       <c r="J20" s="12">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K20" s="12"/>
       <c r="L20" s="16"/>
     </row>
     <row r="21" spans="2:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
-        <f t="shared" si="2"/>
+        <f>B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1689,14 +1701,14 @@
         <v>48</v>
       </c>
       <c r="E21" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H21))-LEN(SUBSTITUTE(TRIM(H21),",",""))+1</f>
         <v>42</v>
       </c>
       <c r="F21" s="11">
         <v>0.1</v>
       </c>
       <c r="G21" s="11">
-        <f t="shared" si="1"/>
+        <f>E21*F21</f>
         <v>4.2</v>
       </c>
       <c r="H21" s="22" t="s">
@@ -1713,7 +1725,7 @@
     </row>
     <row r="22" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
-        <f t="shared" si="2"/>
+        <f>B21+1</f>
         <v>20</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1723,14 +1735,14 @@
         <v>104</v>
       </c>
       <c r="E22" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H22))-LEN(SUBSTITUTE(TRIM(H22),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F22" s="11">
         <v>0.28999999999999998</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" si="1"/>
+        <f>E22*F22</f>
         <v>0.28999999999999998</v>
       </c>
       <c r="H22" s="22" t="s">
@@ -1747,8 +1759,8 @@
     </row>
     <row r="23" spans="2:12" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>B21+1</f>
+        <v>20</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>51</v>
@@ -1757,7 +1769,7 @@
         <v>52</v>
       </c>
       <c r="E23" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H23))-LEN(SUBSTITUTE(TRIM(H23),",",""))+1</f>
         <v>68</v>
       </c>
       <c r="F23" s="11"/>
@@ -1772,222 +1784,248 @@
     </row>
     <row r="24" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f>B23+1</f>
+        <v>21</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>LEN(TRIM(H24))-LEN(SUBSTITUTE(TRIM(H24),",",""))+1</f>
+        <v>1</v>
       </c>
       <c r="F24" s="11">
-        <v>0.4</v>
+        <v>0.73</v>
       </c>
       <c r="G24" s="11">
         <f>E24*F24</f>
-        <v>1.2000000000000002</v>
+        <v>0.73</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>78</v>
+        <v>117</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>118</v>
       </c>
       <c r="J24" s="12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="16"/>
     </row>
-    <row r="25" spans="2:12" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
-        <f t="shared" si="2"/>
-        <v>23</v>
+        <f>B24+1</f>
+        <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E25" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>LEN(TRIM(H25))-LEN(SUBSTITUTE(TRIM(H25),",",""))+1</f>
+        <v>3</v>
       </c>
       <c r="F25" s="11">
-        <v>0.49</v>
+        <v>0.4</v>
       </c>
       <c r="G25" s="11">
         <f>E25*F25</f>
+        <v>1.2000000000000002</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" s="12">
+        <v>6</v>
+      </c>
+      <c r="K25" s="12"/>
+      <c r="L25" s="16"/>
+    </row>
+    <row r="26" spans="2:12" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <f>B25+1</f>
+        <v>23</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="8">
+        <f>LEN(TRIM(H26))-LEN(SUBSTITUTE(TRIM(H26),",",""))+1</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="11">
         <v>0.49</v>
-      </c>
-      <c r="H25" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="I25" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J25" s="12">
-        <v>0</v>
-      </c>
-      <c r="K25" s="12">
-        <v>3</v>
-      </c>
-      <c r="L25" s="16"/>
-    </row>
-    <row r="26" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="8">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E26" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F26" s="11">
-        <v>2.94</v>
       </c>
       <c r="G26" s="11">
         <f>E26*F26</f>
-        <v>2.94</v>
+        <v>0.49</v>
       </c>
       <c r="H26" s="22" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J26" s="12">
         <v>0</v>
       </c>
       <c r="K26" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L26" s="16"/>
     </row>
-    <row r="27" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
-        <f t="shared" si="2"/>
-        <v>25</v>
+        <f>B26+1</f>
+        <v>24</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H27))-LEN(SUBSTITUTE(TRIM(H27),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F27" s="11">
-        <v>1.45</v>
+        <v>2.94</v>
       </c>
       <c r="G27" s="11">
         <f>E27*F27</f>
-        <v>1.45</v>
+        <v>2.94</v>
       </c>
       <c r="H27" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="25" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="I27" s="24" t="s">
+        <v>60</v>
       </c>
       <c r="J27" s="12">
         <v>0</v>
       </c>
       <c r="K27" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L27" s="16"/>
     </row>
     <row r="28" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>B27+1</f>
+        <v>25</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="E28" s="8">
-        <f t="shared" si="0"/>
+        <f>LEN(TRIM(H28))-LEN(SUBSTITUTE(TRIM(H28),",",""))+1</f>
         <v>1</v>
       </c>
       <c r="F28" s="11">
-        <v>1</v>
+        <v>1.45</v>
       </c>
       <c r="G28" s="11">
         <f>E28*F28</f>
+        <v>1.45</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="12">
+        <v>3</v>
+      </c>
+      <c r="L28" s="16"/>
+    </row>
+    <row r="29" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <f>B28+1</f>
+        <v>26</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" s="8">
+        <f>LEN(TRIM(H29))-LEN(SUBSTITUTE(TRIM(H29),",",""))+1</f>
         <v>1</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+      <c r="G29" s="11">
+        <f>E29*F29</f>
+        <v>1</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="24" t="s">
+      <c r="I29" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="J28" s="12">
+      <c r="J29" s="12">
         <v>2</v>
       </c>
-      <c r="K28" s="12">
+      <c r="K29" s="12">
         <v>1</v>
       </c>
-      <c r="L28" s="16"/>
-    </row>
-    <row r="29" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
       <c r="L29" s="16"/>
     </row>
     <row r="30" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C30" s="10"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="11">
-        <f>SUM(G3:G28)</f>
-        <v>22.823999999999995</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
       <c r="L30" s="16"/>
     </row>
-    <row r="31" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="15"/>
+    <row r="31" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11">
+        <f>SUM(G3:G29)</f>
+        <v>23.453999999999997</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
       <c r="L31" s="16"/>
     </row>
     <row r="32" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="18"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
       <c r="K32" s="15"/>
       <c r="L32" s="16"/>
     </row>
@@ -2009,12 +2047,13 @@
     </row>
     <row r="35" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="18"/>
-      <c r="E35" s="18"/>
       <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="21"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="15"/>
+      <c r="L35" s="16"/>
+    </row>
+    <row r="36" spans="2:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19"/>
@@ -2058,8 +2097,6 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="18"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
       <c r="E42" s="18"/>
       <c r="F42" s="19"/>
       <c r="G42" s="19"/>
@@ -2245,38 +2282,48 @@
       <c r="G62" s="19"/>
       <c r="H62" s="21"/>
     </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="18"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="21"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J62">
-    <sortCondition ref="H1"/>
+  <sortState ref="B3:K63">
+    <sortCondition ref="H13"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="I6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="I9" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="I11" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="I12" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="I16" r:id="rId8" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="I15" r:id="rId9" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="I20" r:id="rId10" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="I14" r:id="rId11" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="I25" r:id="rId12" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="I26" r:id="rId13" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="I28" r:id="rId14" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="I18" r:id="rId15" xr:uid="{82C0B133-3910-4F24-8B86-4037327178B9}"/>
-    <hyperlink ref="I19" r:id="rId16" xr:uid="{6D2E285B-37C7-437F-8FAD-5571A7FAFDFB}"/>
-    <hyperlink ref="I21" r:id="rId17" xr:uid="{54FAB168-E422-4A09-97F0-10E4F6F3C922}"/>
-    <hyperlink ref="I22" r:id="rId18" xr:uid="{3118C977-D82B-43D5-9AE9-F41612B3A003}"/>
-    <hyperlink ref="I7" r:id="rId19" xr:uid="{A5375BEB-9BE5-4895-86A9-9E106631B21D}"/>
-    <hyperlink ref="I8" r:id="rId20" xr:uid="{9F8F4839-703E-4F6B-93F2-0DCCC2E8C360}"/>
-    <hyperlink ref="I24" r:id="rId21" xr:uid="{80926A6D-91CC-43D5-9B3D-6C3F296D59C2}"/>
-    <hyperlink ref="I27" r:id="rId22" xr:uid="{CFB56EBC-3D7F-4932-A4E6-91CD1D5FEFDD}"/>
-    <hyperlink ref="I10" r:id="rId23" xr:uid="{D79E5C70-0A8F-472E-B662-FFE8131544D1}"/>
-    <hyperlink ref="I17" r:id="rId24" xr:uid="{8114F172-763A-4E59-930E-B2CFF71CAA31}"/>
-    <hyperlink ref="I13" r:id="rId25" xr:uid="{41FF3E18-7961-452C-B14C-414E7A21BB3F}"/>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="I6" r:id="rId2"/>
+    <hyperlink ref="I4" r:id="rId3"/>
+    <hyperlink ref="I5" r:id="rId4"/>
+    <hyperlink ref="I8" r:id="rId5"/>
+    <hyperlink ref="I12" r:id="rId6"/>
+    <hyperlink ref="I13" r:id="rId7"/>
+    <hyperlink ref="I17" r:id="rId8"/>
+    <hyperlink ref="I16" r:id="rId9"/>
+    <hyperlink ref="I18" r:id="rId10"/>
+    <hyperlink ref="I19" r:id="rId11"/>
+    <hyperlink ref="I26" r:id="rId12"/>
+    <hyperlink ref="I27" r:id="rId13"/>
+    <hyperlink ref="I29" r:id="rId14"/>
+    <hyperlink ref="I20" r:id="rId15"/>
+    <hyperlink ref="I15" r:id="rId16"/>
+    <hyperlink ref="I21" r:id="rId17"/>
+    <hyperlink ref="I22" r:id="rId18"/>
+    <hyperlink ref="I7" r:id="rId19"/>
+    <hyperlink ref="I9" r:id="rId20"/>
+    <hyperlink ref="I25" r:id="rId21"/>
+    <hyperlink ref="I28" r:id="rId22"/>
+    <hyperlink ref="I11" r:id="rId23"/>
+    <hyperlink ref="I14" r:id="rId24"/>
+    <hyperlink ref="I10" r:id="rId25"/>
+    <hyperlink ref="I24" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId26"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>